<commit_message>
Added new attribute - total revenue
</commit_message>
<xml_diff>
--- a/merged_companies.xlsx
+++ b/merged_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I201"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,17 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>TotalRevenue</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>Full Earnings</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Full Revenue</t>
         </is>
       </c>
     </row>
@@ -511,7 +521,13 @@
         <v>117908112000</v>
       </c>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="b">
+      <c r="I2" t="n">
+        <v>1208698287000</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -544,7 +560,13 @@
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="b">
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -581,7 +603,13 @@
       <c r="H4" t="n">
         <v>45614.26</v>
       </c>
-      <c r="I4" t="b">
+      <c r="I4" t="n">
+        <v>284411845357</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -618,7 +646,13 @@
       <c r="H5" t="n">
         <v>303598.73</v>
       </c>
-      <c r="I5" t="b">
+      <c r="I5" t="n">
+        <v>255477482883</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -651,7 +685,13 @@
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="b">
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -684,7 +724,13 @@
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="b">
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -717,7 +763,13 @@
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
-      <c r="I8" t="b">
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -750,7 +802,13 @@
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
-      <c r="I9" t="b">
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -785,7 +843,13 @@
         <v>18014467405</v>
       </c>
       <c r="H10" t="inlineStr"/>
-      <c r="I10" t="b">
+      <c r="I10" t="n">
+        <v>150413333210</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -818,7 +882,13 @@
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="b">
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -851,7 +921,13 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
-      <c r="I12" t="b">
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -884,7 +960,13 @@
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="b">
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -921,7 +1003,13 @@
       <c r="H14" t="n">
         <v>63615.09</v>
       </c>
-      <c r="I14" t="b">
+      <c r="I14" t="n">
+        <v>32164260254</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
         <v>1</v>
       </c>
     </row>
@@ -956,7 +1044,13 @@
       <c r="H15" t="n">
         <v>489642.56</v>
       </c>
-      <c r="I15" t="b">
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -993,7 +1087,13 @@
       <c r="H16" t="n">
         <v>167581.76</v>
       </c>
-      <c r="I16" t="b">
+      <c r="I16" t="n">
+        <v>147419453323</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1026,7 +1126,13 @@
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="b">
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1061,7 +1167,13 @@
       <c r="H18" t="n">
         <v>149505.68</v>
       </c>
-      <c r="I18" t="b">
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1098,7 +1210,13 @@
       <c r="H19" t="n">
         <v>183883.65</v>
       </c>
-      <c r="I19" t="b">
+      <c r="I19" t="n">
+        <v>62962652135</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1133,7 +1251,13 @@
       <c r="H20" t="n">
         <v>258035.05</v>
       </c>
-      <c r="I20" t="b">
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1168,7 +1292,13 @@
       <c r="H21" t="n">
         <v>211846.17</v>
       </c>
-      <c r="I21" t="b">
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1203,7 +1333,13 @@
       <c r="H22" t="n">
         <v>149554.46</v>
       </c>
-      <c r="I22" t="b">
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1236,7 +1372,13 @@
       </c>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="b">
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1269,7 +1411,13 @@
       </c>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr"/>
-      <c r="I24" t="b">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1302,7 +1450,13 @@
       </c>
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr"/>
-      <c r="I25" t="b">
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1337,7 +1491,13 @@
       <c r="H26" t="n">
         <v>110996.45</v>
       </c>
-      <c r="I26" t="b">
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1370,7 +1530,13 @@
       </c>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
-      <c r="I27" t="b">
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1407,7 +1573,13 @@
       <c r="H28" t="n">
         <v>89753.14</v>
       </c>
-      <c r="I28" t="b">
+      <c r="I28" t="n">
+        <v>83460489000</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1440,7 +1612,13 @@
       </c>
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr"/>
-      <c r="I29" t="b">
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1473,7 +1651,13 @@
       </c>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="b">
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1510,7 +1694,13 @@
       <c r="H31" t="n">
         <v>117455.5</v>
       </c>
-      <c r="I31" t="b">
+      <c r="I31" t="n">
+        <v>61823889923</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1543,7 +1733,13 @@
       </c>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
-      <c r="I32" t="b">
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1580,7 +1776,13 @@
       <c r="H33" t="n">
         <v>212688.06</v>
       </c>
-      <c r="I33" t="b">
+      <c r="I33" t="n">
+        <v>23366300997</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1617,7 +1819,13 @@
       <c r="H34" t="n">
         <v>8379.57</v>
       </c>
-      <c r="I34" t="b">
+      <c r="I34" t="n">
+        <v>8459192465</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1650,7 +1858,13 @@
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr"/>
-      <c r="I35" t="b">
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1683,7 +1897,13 @@
       </c>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr"/>
-      <c r="I36" t="b">
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1716,7 +1936,13 @@
       </c>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr"/>
-      <c r="I37" t="b">
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1745,7 +1971,11 @@
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr"/>
-      <c r="I38" t="b">
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1782,7 +2012,13 @@
       <c r="H39" t="n">
         <v>76175.16</v>
       </c>
-      <c r="I39" t="b">
+      <c r="I39" t="n">
+        <v>109144878896</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1817,7 +2053,13 @@
       <c r="H40" t="n">
         <v>54220.13</v>
       </c>
-      <c r="I40" t="b">
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1854,7 +2096,13 @@
       <c r="H41" t="n">
         <v>1466.8</v>
       </c>
-      <c r="I41" t="b">
+      <c r="I41" t="n">
+        <v>20413120644</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1889,7 +2137,13 @@
       <c r="H42" t="n">
         <v>52848.26</v>
       </c>
-      <c r="I42" t="b">
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1922,7 +2176,13 @@
       </c>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
-      <c r="I43" t="b">
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1955,7 +2215,13 @@
       </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr"/>
-      <c r="I44" t="b">
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1988,7 +2254,13 @@
       </c>
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr"/>
-      <c r="I45" t="b">
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2021,7 +2293,13 @@
       </c>
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr"/>
-      <c r="I46" t="b">
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2054,7 +2332,13 @@
       </c>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr"/>
-      <c r="I47" t="b">
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2089,7 +2373,13 @@
       <c r="H48" t="n">
         <v>36194.8</v>
       </c>
-      <c r="I48" t="b">
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2122,7 +2412,13 @@
       </c>
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr"/>
-      <c r="I49" t="b">
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2155,7 +2451,13 @@
       </c>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr"/>
-      <c r="I50" t="b">
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2188,7 +2490,13 @@
       </c>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr"/>
-      <c r="I51" t="b">
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2221,7 +2529,13 @@
       </c>
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr"/>
-      <c r="I52" t="b">
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2254,7 +2568,13 @@
       </c>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
-      <c r="I53" t="b">
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2287,7 +2607,13 @@
       </c>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="b">
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2320,7 +2646,13 @@
       </c>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="b">
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2355,7 +2687,13 @@
       <c r="H56" t="n">
         <v>75408.63</v>
       </c>
-      <c r="I56" t="b">
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2388,7 +2726,13 @@
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="b">
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2421,7 +2765,13 @@
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="b">
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2454,7 +2804,13 @@
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="b">
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2487,7 +2843,13 @@
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
-      <c r="I60" t="b">
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J60" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2520,7 +2882,13 @@
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
-      <c r="I61" t="b">
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2553,7 +2921,13 @@
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="b">
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2590,7 +2964,13 @@
       <c r="H63" t="n">
         <v>7546.77</v>
       </c>
-      <c r="I63" t="b">
+      <c r="I63" t="n">
+        <v>1721049617</v>
+      </c>
+      <c r="J63" t="b">
+        <v>1</v>
+      </c>
+      <c r="K63" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2623,7 +3003,13 @@
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
-      <c r="I64" t="b">
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2656,7 +3042,13 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="b">
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2689,7 +3081,13 @@
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="b">
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2722,7 +3120,13 @@
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
-      <c r="I67" t="b">
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2759,7 +3163,13 @@
       <c r="H68" t="n">
         <v>112400</v>
       </c>
-      <c r="I68" t="b">
+      <c r="I68" t="n">
+        <v>26248984718</v>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+      <c r="K68" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2792,7 +3202,13 @@
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
-      <c r="I69" t="b">
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2829,8 +3245,14 @@
       <c r="H70" t="n">
         <v>1100.28</v>
       </c>
-      <c r="I70" t="b">
-        <v>1</v>
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+      <c r="K70" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2862,7 +3284,13 @@
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="b">
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+      <c r="K71" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2897,7 +3325,13 @@
       <c r="H72" t="n">
         <v>30030</v>
       </c>
-      <c r="I72" t="b">
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" t="b">
+        <v>0</v>
+      </c>
+      <c r="K72" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2930,7 +3364,13 @@
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
-      <c r="I73" t="b">
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+      <c r="K73" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2965,7 +3405,13 @@
       <c r="H74" t="n">
         <v>105451.06</v>
       </c>
-      <c r="I74" t="b">
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" t="b">
+        <v>0</v>
+      </c>
+      <c r="K74" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3002,7 +3448,13 @@
       <c r="H75" t="n">
         <v>1295.36</v>
       </c>
-      <c r="I75" t="b">
+      <c r="I75" t="n">
+        <v>2243571977</v>
+      </c>
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+      <c r="K75" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3035,7 +3487,13 @@
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
-      <c r="I76" t="b">
+      <c r="I76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J76" t="b">
+        <v>0</v>
+      </c>
+      <c r="K76" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3068,7 +3526,13 @@
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
-      <c r="I77" t="b">
+      <c r="I77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+      <c r="K77" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3101,7 +3565,13 @@
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
-      <c r="I78" t="b">
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" t="b">
+        <v>0</v>
+      </c>
+      <c r="K78" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3134,7 +3604,13 @@
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
-      <c r="I79" t="b">
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+      <c r="K79" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3167,7 +3643,13 @@
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
-      <c r="I80" t="b">
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" t="b">
+        <v>0</v>
+      </c>
+      <c r="K80" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3196,7 +3678,11 @@
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
-      <c r="I81" t="b">
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+      <c r="K81" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3229,7 +3715,13 @@
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
-      <c r="I82" t="b">
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" t="b">
+        <v>0</v>
+      </c>
+      <c r="K82" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3264,7 +3756,13 @@
         <v>-3062613</v>
       </c>
       <c r="H83" t="inlineStr"/>
-      <c r="I83" t="b">
+      <c r="I83" t="n">
+        <v>3412662</v>
+      </c>
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+      <c r="K83" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3301,7 +3799,13 @@
       <c r="H84" t="n">
         <v>15938.47</v>
       </c>
-      <c r="I84" t="b">
+      <c r="I84" t="n">
+        <v>1281265789</v>
+      </c>
+      <c r="J84" t="b">
+        <v>1</v>
+      </c>
+      <c r="K84" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3336,7 +3840,13 @@
       <c r="H85" t="n">
         <v>36448.05</v>
       </c>
-      <c r="I85" t="b">
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+      <c r="K85" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3373,7 +3883,13 @@
       <c r="H86" t="n">
         <v>28755.73</v>
       </c>
-      <c r="I86" t="b">
+      <c r="I86" t="n">
+        <v>35289598359</v>
+      </c>
+      <c r="J86" t="b">
+        <v>1</v>
+      </c>
+      <c r="K86" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3408,7 +3924,13 @@
         <v>194547912</v>
       </c>
       <c r="H87" t="inlineStr"/>
-      <c r="I87" t="b">
+      <c r="I87" t="n">
+        <v>63311663</v>
+      </c>
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+      <c r="K87" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3445,7 +3967,13 @@
       <c r="H88" t="n">
         <v>33724.56</v>
       </c>
-      <c r="I88" t="b">
+      <c r="I88" t="n">
+        <v>8623963649</v>
+      </c>
+      <c r="J88" t="b">
+        <v>1</v>
+      </c>
+      <c r="K88" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3478,7 +4006,13 @@
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
-      <c r="I89" t="b">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+      <c r="K89" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3511,7 +4045,13 @@
       </c>
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr"/>
-      <c r="I90" t="b">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+      <c r="K90" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3548,7 +4088,13 @@
       <c r="H91" t="n">
         <v>13959</v>
       </c>
-      <c r="I91" t="b">
+      <c r="I91" t="n">
+        <v>8172896486</v>
+      </c>
+      <c r="J91" t="b">
+        <v>1</v>
+      </c>
+      <c r="K91" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3585,7 +4131,13 @@
       <c r="H92" t="n">
         <v>63859.5</v>
       </c>
-      <c r="I92" t="b">
+      <c r="I92" t="n">
+        <v>6265861178</v>
+      </c>
+      <c r="J92" t="b">
+        <v>1</v>
+      </c>
+      <c r="K92" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3622,7 +4174,13 @@
       <c r="H93" t="n">
         <v>94947.50999999999</v>
       </c>
-      <c r="I93" t="b">
+      <c r="I93" t="n">
+        <v>139872996975</v>
+      </c>
+      <c r="J93" t="b">
+        <v>1</v>
+      </c>
+      <c r="K93" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3655,7 +4213,13 @@
       </c>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr"/>
-      <c r="I94" t="b">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" t="b">
+        <v>0</v>
+      </c>
+      <c r="K94" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3688,7 +4252,13 @@
       </c>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="inlineStr"/>
-      <c r="I95" t="b">
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+      <c r="K95" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3725,7 +4295,13 @@
       <c r="H96" t="n">
         <v>1241.62</v>
       </c>
-      <c r="I96" t="b">
+      <c r="I96" t="n">
+        <v>1415451992</v>
+      </c>
+      <c r="J96" t="b">
+        <v>1</v>
+      </c>
+      <c r="K96" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3762,7 +4338,13 @@
       <c r="H97" t="n">
         <v>10000.13</v>
       </c>
-      <c r="I97" t="b">
+      <c r="I97" t="n">
+        <v>9477575304</v>
+      </c>
+      <c r="J97" t="b">
+        <v>1</v>
+      </c>
+      <c r="K97" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3797,7 +4379,13 @@
       <c r="H98" t="n">
         <v>26753.81</v>
       </c>
-      <c r="I98" t="b">
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" t="b">
+        <v>0</v>
+      </c>
+      <c r="K98" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3832,7 +4420,13 @@
       <c r="H99" t="n">
         <v>53486</v>
       </c>
-      <c r="I99" t="b">
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+      <c r="K99" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3869,7 +4463,13 @@
       <c r="H100" t="n">
         <v>13023.85</v>
       </c>
-      <c r="I100" t="b">
+      <c r="I100" t="n">
+        <v>21869458380</v>
+      </c>
+      <c r="J100" t="b">
+        <v>1</v>
+      </c>
+      <c r="K100" t="b">
         <v>1</v>
       </c>
     </row>
@@ -3902,7 +4502,13 @@
       </c>
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr"/>
-      <c r="I101" t="b">
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+      <c r="K101" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3935,7 +4541,13 @@
       </c>
       <c r="G102" t="inlineStr"/>
       <c r="H102" t="inlineStr"/>
-      <c r="I102" t="b">
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" t="b">
+        <v>0</v>
+      </c>
+      <c r="K102" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3972,7 +4584,13 @@
       <c r="H103" t="n">
         <v>46986.85</v>
       </c>
-      <c r="I103" t="b">
+      <c r="I103" t="n">
+        <v>8529279576</v>
+      </c>
+      <c r="J103" t="b">
+        <v>1</v>
+      </c>
+      <c r="K103" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4009,7 +4627,13 @@
       <c r="H104" t="n">
         <v>9625.23</v>
       </c>
-      <c r="I104" t="b">
+      <c r="I104" t="n">
+        <v>40279778659</v>
+      </c>
+      <c r="J104" t="b">
+        <v>1</v>
+      </c>
+      <c r="K104" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4046,7 +4670,13 @@
       <c r="H105" t="n">
         <v>29575.92</v>
       </c>
-      <c r="I105" t="b">
+      <c r="I105" t="n">
+        <v>3295129859</v>
+      </c>
+      <c r="J105" t="b">
+        <v>1</v>
+      </c>
+      <c r="K105" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4083,7 +4713,13 @@
       <c r="H106" t="n">
         <v>16911.82</v>
       </c>
-      <c r="I106" t="b">
+      <c r="I106" t="n">
+        <v>10061554214</v>
+      </c>
+      <c r="J106" t="b">
+        <v>1</v>
+      </c>
+      <c r="K106" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4116,7 +4752,13 @@
       </c>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
-      <c r="I107" t="b">
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" t="b">
+        <v>0</v>
+      </c>
+      <c r="K107" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4153,7 +4795,13 @@
       <c r="H108" t="n">
         <v>23367.3</v>
       </c>
-      <c r="I108" t="b">
+      <c r="I108" t="n">
+        <v>5324411264</v>
+      </c>
+      <c r="J108" t="b">
+        <v>1</v>
+      </c>
+      <c r="K108" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4190,7 +4838,13 @@
       <c r="H109" t="n">
         <v>81880.10000000001</v>
       </c>
-      <c r="I109" t="b">
+      <c r="I109" t="n">
+        <v>17135684754</v>
+      </c>
+      <c r="J109" t="b">
+        <v>1</v>
+      </c>
+      <c r="K109" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4225,7 +4879,13 @@
         <v>1073259464</v>
       </c>
       <c r="H110" t="inlineStr"/>
-      <c r="I110" t="b">
+      <c r="I110" t="n">
+        <v>5151411045</v>
+      </c>
+      <c r="J110" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4262,7 +4922,13 @@
       <c r="H111" t="n">
         <v>23446.73</v>
       </c>
-      <c r="I111" t="b">
+      <c r="I111" t="n">
+        <v>5133914168</v>
+      </c>
+      <c r="J111" t="b">
+        <v>1</v>
+      </c>
+      <c r="K111" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4299,7 +4965,13 @@
       <c r="H112" t="n">
         <v>2820</v>
       </c>
-      <c r="I112" t="b">
+      <c r="I112" t="n">
+        <v>1318816864</v>
+      </c>
+      <c r="J112" t="b">
+        <v>1</v>
+      </c>
+      <c r="K112" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4336,7 +5008,13 @@
       <c r="H113" t="n">
         <v>223.32</v>
       </c>
-      <c r="I113" t="b">
+      <c r="I113" t="n">
+        <v>704425452</v>
+      </c>
+      <c r="J113" t="b">
+        <v>1</v>
+      </c>
+      <c r="K113" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4369,7 +5047,13 @@
       </c>
       <c r="G114" t="inlineStr"/>
       <c r="H114" t="inlineStr"/>
-      <c r="I114" t="b">
+      <c r="I114" t="n">
+        <v>0</v>
+      </c>
+      <c r="J114" t="b">
+        <v>0</v>
+      </c>
+      <c r="K114" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4406,7 +5090,13 @@
       <c r="H115" t="n">
         <v>48853.34</v>
       </c>
-      <c r="I115" t="b">
+      <c r="I115" t="n">
+        <v>71976618920</v>
+      </c>
+      <c r="J115" t="b">
+        <v>1</v>
+      </c>
+      <c r="K115" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4439,7 +5129,13 @@
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="b">
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" t="b">
+        <v>0</v>
+      </c>
+      <c r="K116" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4468,7 +5164,11 @@
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
-      <c r="I117" t="b">
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="b">
+        <v>0</v>
+      </c>
+      <c r="K117" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4501,7 +5201,13 @@
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
-      <c r="I118" t="b">
+      <c r="I118" t="n">
+        <v>0</v>
+      </c>
+      <c r="J118" t="b">
+        <v>0</v>
+      </c>
+      <c r="K118" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4536,7 +5242,13 @@
       <c r="H119" t="n">
         <v>36788.73</v>
       </c>
-      <c r="I119" t="b">
+      <c r="I119" t="n">
+        <v>0</v>
+      </c>
+      <c r="J119" t="b">
+        <v>0</v>
+      </c>
+      <c r="K119" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4569,7 +5281,11 @@
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="b">
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="b">
+        <v>0</v>
+      </c>
+      <c r="K120" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4606,7 +5322,13 @@
       <c r="H121" t="n">
         <v>23888.78</v>
       </c>
-      <c r="I121" t="b">
+      <c r="I121" t="n">
+        <v>9041607472</v>
+      </c>
+      <c r="J121" t="b">
+        <v>1</v>
+      </c>
+      <c r="K121" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4643,7 +5365,13 @@
       <c r="H122" t="n">
         <v>35661.19</v>
       </c>
-      <c r="I122" t="b">
+      <c r="I122" t="n">
+        <v>10296575481</v>
+      </c>
+      <c r="J122" t="b">
+        <v>1</v>
+      </c>
+      <c r="K122" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4680,7 +5408,13 @@
       <c r="H123" t="n">
         <v>12899.69</v>
       </c>
-      <c r="I123" t="b">
+      <c r="I123" t="n">
+        <v>12804804439</v>
+      </c>
+      <c r="J123" t="b">
+        <v>1</v>
+      </c>
+      <c r="K123" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4713,7 +5447,13 @@
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
-      <c r="I124" t="b">
+      <c r="I124" t="n">
+        <v>0</v>
+      </c>
+      <c r="J124" t="b">
+        <v>0</v>
+      </c>
+      <c r="K124" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4750,7 +5490,13 @@
       <c r="H125" t="n">
         <v>25009.41</v>
       </c>
-      <c r="I125" t="b">
+      <c r="I125" t="n">
+        <v>35406142984</v>
+      </c>
+      <c r="J125" t="b">
+        <v>1</v>
+      </c>
+      <c r="K125" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4785,7 +5531,13 @@
       <c r="H126" t="n">
         <v>22814</v>
       </c>
-      <c r="I126" t="b">
+      <c r="I126" t="n">
+        <v>0</v>
+      </c>
+      <c r="J126" t="b">
+        <v>0</v>
+      </c>
+      <c r="K126" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4818,7 +5570,13 @@
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr"/>
-      <c r="I127" t="b">
+      <c r="I127" t="n">
+        <v>0</v>
+      </c>
+      <c r="J127" t="b">
+        <v>0</v>
+      </c>
+      <c r="K127" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4847,7 +5605,11 @@
       </c>
       <c r="G128" t="inlineStr"/>
       <c r="H128" t="inlineStr"/>
-      <c r="I128" t="b">
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" t="b">
+        <v>0</v>
+      </c>
+      <c r="K128" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4884,7 +5646,13 @@
       <c r="H129" t="n">
         <v>8451.299999999999</v>
       </c>
-      <c r="I129" t="b">
+      <c r="I129" t="n">
+        <v>5534899642</v>
+      </c>
+      <c r="J129" t="b">
+        <v>1</v>
+      </c>
+      <c r="K129" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4917,7 +5685,13 @@
       </c>
       <c r="G130" t="inlineStr"/>
       <c r="H130" t="inlineStr"/>
-      <c r="I130" t="b">
+      <c r="I130" t="n">
+        <v>0</v>
+      </c>
+      <c r="J130" t="b">
+        <v>0</v>
+      </c>
+      <c r="K130" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4954,7 +5728,13 @@
       <c r="H131" t="n">
         <v>4881.6</v>
       </c>
-      <c r="I131" t="b">
+      <c r="I131" t="n">
+        <v>39014921936</v>
+      </c>
+      <c r="J131" t="b">
+        <v>1</v>
+      </c>
+      <c r="K131" t="b">
         <v>1</v>
       </c>
     </row>
@@ -4987,7 +5767,13 @@
       </c>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="inlineStr"/>
-      <c r="I132" t="b">
+      <c r="I132" t="n">
+        <v>0</v>
+      </c>
+      <c r="J132" t="b">
+        <v>0</v>
+      </c>
+      <c r="K132" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5020,7 +5806,13 @@
       </c>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
-      <c r="I133" t="b">
+      <c r="I133" t="n">
+        <v>0</v>
+      </c>
+      <c r="J133" t="b">
+        <v>0</v>
+      </c>
+      <c r="K133" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5057,7 +5849,13 @@
       <c r="H134" t="n">
         <v>12424.23</v>
       </c>
-      <c r="I134" t="b">
+      <c r="I134" t="n">
+        <v>6199498811</v>
+      </c>
+      <c r="J134" t="b">
+        <v>1</v>
+      </c>
+      <c r="K134" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5094,7 +5892,13 @@
       <c r="H135" t="n">
         <v>7957.54</v>
       </c>
-      <c r="I135" t="b">
+      <c r="I135" t="n">
+        <v>10027765814</v>
+      </c>
+      <c r="J135" t="b">
+        <v>1</v>
+      </c>
+      <c r="K135" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5131,7 +5935,13 @@
       <c r="H136" t="n">
         <v>2567.94</v>
       </c>
-      <c r="I136" t="b">
+      <c r="I136" t="n">
+        <v>792383106</v>
+      </c>
+      <c r="J136" t="b">
+        <v>1</v>
+      </c>
+      <c r="K136" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5164,7 +5974,13 @@
       </c>
       <c r="G137" t="inlineStr"/>
       <c r="H137" t="inlineStr"/>
-      <c r="I137" t="b">
+      <c r="I137" t="n">
+        <v>0</v>
+      </c>
+      <c r="J137" t="b">
+        <v>0</v>
+      </c>
+      <c r="K137" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5201,7 +6017,13 @@
       <c r="H138" t="n">
         <v>18935.24</v>
       </c>
-      <c r="I138" t="b">
+      <c r="I138" t="n">
+        <v>4276240392</v>
+      </c>
+      <c r="J138" t="b">
+        <v>1</v>
+      </c>
+      <c r="K138" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5238,7 +6060,13 @@
       <c r="H139" t="n">
         <v>1052.15</v>
       </c>
-      <c r="I139" t="b">
+      <c r="I139" t="n">
+        <v>17637444688</v>
+      </c>
+      <c r="J139" t="b">
+        <v>1</v>
+      </c>
+      <c r="K139" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5273,7 +6101,13 @@
       <c r="H140" t="n">
         <v>1081.5</v>
       </c>
-      <c r="I140" t="b">
+      <c r="I140" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" t="b">
+        <v>0</v>
+      </c>
+      <c r="K140" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5306,7 +6140,13 @@
       </c>
       <c r="G141" t="inlineStr"/>
       <c r="H141" t="inlineStr"/>
-      <c r="I141" t="b">
+      <c r="I141" t="n">
+        <v>0</v>
+      </c>
+      <c r="J141" t="b">
+        <v>0</v>
+      </c>
+      <c r="K141" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5339,7 +6179,13 @@
       </c>
       <c r="G142" t="inlineStr"/>
       <c r="H142" t="inlineStr"/>
-      <c r="I142" t="b">
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="b">
+        <v>0</v>
+      </c>
+      <c r="K142" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5376,7 +6222,13 @@
       <c r="H143" t="n">
         <v>6971.24</v>
       </c>
-      <c r="I143" t="b">
+      <c r="I143" t="n">
+        <v>1344706054</v>
+      </c>
+      <c r="J143" t="b">
+        <v>1</v>
+      </c>
+      <c r="K143" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5409,7 +6261,13 @@
       </c>
       <c r="G144" t="inlineStr"/>
       <c r="H144" t="inlineStr"/>
-      <c r="I144" t="b">
+      <c r="I144" t="n">
+        <v>0</v>
+      </c>
+      <c r="J144" t="b">
+        <v>0</v>
+      </c>
+      <c r="K144" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5442,7 +6300,13 @@
       </c>
       <c r="G145" t="inlineStr"/>
       <c r="H145" t="inlineStr"/>
-      <c r="I145" t="b">
+      <c r="I145" t="n">
+        <v>0</v>
+      </c>
+      <c r="J145" t="b">
+        <v>0</v>
+      </c>
+      <c r="K145" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5475,7 +6339,13 @@
       </c>
       <c r="G146" t="inlineStr"/>
       <c r="H146" t="inlineStr"/>
-      <c r="I146" t="b">
+      <c r="I146" t="n">
+        <v>0</v>
+      </c>
+      <c r="J146" t="b">
+        <v>0</v>
+      </c>
+      <c r="K146" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5512,7 +6382,13 @@
       <c r="H147" t="n">
         <v>2449.27</v>
       </c>
-      <c r="I147" t="b">
+      <c r="I147" t="n">
+        <v>19584901776</v>
+      </c>
+      <c r="J147" t="b">
+        <v>1</v>
+      </c>
+      <c r="K147" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5549,7 +6425,13 @@
       <c r="H148" t="n">
         <v>2359.45</v>
       </c>
-      <c r="I148" t="b">
+      <c r="I148" t="n">
+        <v>8413912097</v>
+      </c>
+      <c r="J148" t="b">
+        <v>1</v>
+      </c>
+      <c r="K148" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5582,7 +6464,13 @@
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="inlineStr"/>
-      <c r="I149" t="b">
+      <c r="I149" t="n">
+        <v>0</v>
+      </c>
+      <c r="J149" t="b">
+        <v>0</v>
+      </c>
+      <c r="K149" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5619,7 +6507,13 @@
       <c r="H150" t="n">
         <v>14091.63</v>
       </c>
-      <c r="I150" t="b">
+      <c r="I150" t="n">
+        <v>31190353611</v>
+      </c>
+      <c r="J150" t="b">
+        <v>1</v>
+      </c>
+      <c r="K150" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5652,7 +6546,13 @@
       </c>
       <c r="G151" t="inlineStr"/>
       <c r="H151" t="inlineStr"/>
-      <c r="I151" t="b">
+      <c r="I151" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" t="b">
+        <v>0</v>
+      </c>
+      <c r="K151" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5689,7 +6589,13 @@
       <c r="H152" t="n">
         <v>8290.57</v>
       </c>
-      <c r="I152" t="b">
+      <c r="I152" t="n">
+        <v>2561535403</v>
+      </c>
+      <c r="J152" t="b">
+        <v>1</v>
+      </c>
+      <c r="K152" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5726,7 +6632,13 @@
       <c r="H153" t="n">
         <v>5250</v>
       </c>
-      <c r="I153" t="b">
+      <c r="I153" t="n">
+        <v>17831082882</v>
+      </c>
+      <c r="J153" t="b">
+        <v>1</v>
+      </c>
+      <c r="K153" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5763,7 +6675,13 @@
       <c r="H154" t="n">
         <v>16229.15</v>
       </c>
-      <c r="I154" t="b">
+      <c r="I154" t="n">
+        <v>8899589311</v>
+      </c>
+      <c r="J154" t="b">
+        <v>1</v>
+      </c>
+      <c r="K154" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5800,7 +6718,13 @@
       <c r="H155" t="n">
         <v>1387.12</v>
       </c>
-      <c r="I155" t="b">
+      <c r="I155" t="n">
+        <v>7359354990</v>
+      </c>
+      <c r="J155" t="b">
+        <v>1</v>
+      </c>
+      <c r="K155" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5837,7 +6761,13 @@
       <c r="H156" t="n">
         <v>7606.83</v>
       </c>
-      <c r="I156" t="b">
+      <c r="I156" t="n">
+        <v>7508833947</v>
+      </c>
+      <c r="J156" t="b">
+        <v>1</v>
+      </c>
+      <c r="K156" t="b">
         <v>1</v>
       </c>
     </row>
@@ -5870,7 +6800,13 @@
       </c>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="inlineStr"/>
-      <c r="I157" t="b">
+      <c r="I157" t="n">
+        <v>0</v>
+      </c>
+      <c r="J157" t="b">
+        <v>0</v>
+      </c>
+      <c r="K157" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5903,7 +6839,13 @@
       </c>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="inlineStr"/>
-      <c r="I158" t="b">
+      <c r="I158" t="n">
+        <v>0</v>
+      </c>
+      <c r="J158" t="b">
+        <v>0</v>
+      </c>
+      <c r="K158" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5938,7 +6880,13 @@
       <c r="H159" t="n">
         <v>2580.67</v>
       </c>
-      <c r="I159" t="b">
+      <c r="I159" t="n">
+        <v>0</v>
+      </c>
+      <c r="J159" t="b">
+        <v>0</v>
+      </c>
+      <c r="K159" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5971,7 +6919,13 @@
       </c>
       <c r="G160" t="inlineStr"/>
       <c r="H160" t="inlineStr"/>
-      <c r="I160" t="b">
+      <c r="I160" t="n">
+        <v>0</v>
+      </c>
+      <c r="J160" t="b">
+        <v>0</v>
+      </c>
+      <c r="K160" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6004,7 +6958,13 @@
       </c>
       <c r="G161" t="inlineStr"/>
       <c r="H161" t="inlineStr"/>
-      <c r="I161" t="b">
+      <c r="I161" t="n">
+        <v>0</v>
+      </c>
+      <c r="J161" t="b">
+        <v>0</v>
+      </c>
+      <c r="K161" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6041,7 +7001,13 @@
       <c r="H162" t="n">
         <v>27072.35</v>
       </c>
-      <c r="I162" t="b">
+      <c r="I162" t="n">
+        <v>3695525336</v>
+      </c>
+      <c r="J162" t="b">
+        <v>1</v>
+      </c>
+      <c r="K162" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6074,7 +7040,13 @@
       </c>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr"/>
-      <c r="I163" t="b">
+      <c r="I163" t="n">
+        <v>0</v>
+      </c>
+      <c r="J163" t="b">
+        <v>0</v>
+      </c>
+      <c r="K163" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6107,7 +7079,13 @@
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="inlineStr"/>
-      <c r="I164" t="b">
+      <c r="I164" t="n">
+        <v>0</v>
+      </c>
+      <c r="J164" t="b">
+        <v>0</v>
+      </c>
+      <c r="K164" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6144,7 +7122,13 @@
       <c r="H165" t="n">
         <v>1575.49</v>
       </c>
-      <c r="I165" t="b">
+      <c r="I165" t="n">
+        <v>14199068821</v>
+      </c>
+      <c r="J165" t="b">
+        <v>1</v>
+      </c>
+      <c r="K165" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6181,7 +7165,13 @@
       <c r="H166" t="n">
         <v>2895.89</v>
       </c>
-      <c r="I166" t="b">
+      <c r="I166" t="n">
+        <v>4733156444</v>
+      </c>
+      <c r="J166" t="b">
+        <v>1</v>
+      </c>
+      <c r="K166" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6214,7 +7204,13 @@
       </c>
       <c r="G167" t="inlineStr"/>
       <c r="H167" t="inlineStr"/>
-      <c r="I167" t="b">
+      <c r="I167" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" t="b">
+        <v>0</v>
+      </c>
+      <c r="K167" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6251,7 +7247,13 @@
       <c r="H168" t="n">
         <v>12187.81</v>
       </c>
-      <c r="I168" t="b">
+      <c r="I168" t="n">
+        <v>12383063413</v>
+      </c>
+      <c r="J168" t="b">
+        <v>1</v>
+      </c>
+      <c r="K168" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6288,7 +7290,13 @@
       <c r="H169" t="n">
         <v>7745.3</v>
       </c>
-      <c r="I169" t="b">
+      <c r="I169" t="n">
+        <v>12425473708</v>
+      </c>
+      <c r="J169" t="b">
+        <v>1</v>
+      </c>
+      <c r="K169" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6325,7 +7333,13 @@
       <c r="H170" t="n">
         <v>15105.46</v>
       </c>
-      <c r="I170" t="b">
+      <c r="I170" t="n">
+        <v>2292832702</v>
+      </c>
+      <c r="J170" t="b">
+        <v>1</v>
+      </c>
+      <c r="K170" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6360,7 +7374,13 @@
       <c r="H171" t="n">
         <v>7866.28</v>
       </c>
-      <c r="I171" t="b">
+      <c r="I171" t="n">
+        <v>0</v>
+      </c>
+      <c r="J171" t="b">
+        <v>0</v>
+      </c>
+      <c r="K171" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6393,7 +7413,13 @@
       </c>
       <c r="G172" t="inlineStr"/>
       <c r="H172" t="inlineStr"/>
-      <c r="I172" t="b">
+      <c r="I172" t="n">
+        <v>0</v>
+      </c>
+      <c r="J172" t="b">
+        <v>0</v>
+      </c>
+      <c r="K172" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6426,7 +7452,13 @@
       </c>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="inlineStr"/>
-      <c r="I173" t="b">
+      <c r="I173" t="n">
+        <v>0</v>
+      </c>
+      <c r="J173" t="b">
+        <v>0</v>
+      </c>
+      <c r="K173" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6463,7 +7495,13 @@
       <c r="H174" t="n">
         <v>14042.13</v>
       </c>
-      <c r="I174" t="b">
+      <c r="I174" t="n">
+        <v>5647936253</v>
+      </c>
+      <c r="J174" t="b">
+        <v>1</v>
+      </c>
+      <c r="K174" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6500,7 +7538,13 @@
       <c r="H175" t="n">
         <v>13596.98</v>
       </c>
-      <c r="I175" t="b">
+      <c r="I175" t="n">
+        <v>8039546309</v>
+      </c>
+      <c r="J175" t="b">
+        <v>1</v>
+      </c>
+      <c r="K175" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6537,7 +7581,13 @@
       <c r="H176" t="n">
         <v>1307.4</v>
       </c>
-      <c r="I176" t="b">
+      <c r="I176" t="n">
+        <v>4659712532</v>
+      </c>
+      <c r="J176" t="b">
+        <v>1</v>
+      </c>
+      <c r="K176" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6572,7 +7622,13 @@
         <v>4122446</v>
       </c>
       <c r="H177" t="inlineStr"/>
-      <c r="I177" t="b">
+      <c r="I177" t="n">
+        <v>323968946</v>
+      </c>
+      <c r="J177" t="b">
+        <v>1</v>
+      </c>
+      <c r="K177" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6609,7 +7665,13 @@
       <c r="H178" t="n">
         <v>125</v>
       </c>
-      <c r="I178" t="b">
+      <c r="I178" t="n">
+        <v>394164626</v>
+      </c>
+      <c r="J178" t="b">
+        <v>1</v>
+      </c>
+      <c r="K178" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6642,7 +7704,13 @@
       </c>
       <c r="G179" t="inlineStr"/>
       <c r="H179" t="inlineStr"/>
-      <c r="I179" t="b">
+      <c r="I179" t="n">
+        <v>0</v>
+      </c>
+      <c r="J179" t="b">
+        <v>0</v>
+      </c>
+      <c r="K179" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6679,7 +7747,13 @@
       <c r="H180" t="n">
         <v>14369.02</v>
       </c>
-      <c r="I180" t="b">
+      <c r="I180" t="n">
+        <v>4597064189</v>
+      </c>
+      <c r="J180" t="b">
+        <v>1</v>
+      </c>
+      <c r="K180" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6714,7 +7788,13 @@
       <c r="H181" t="n">
         <v>10538.24</v>
       </c>
-      <c r="I181" t="b">
+      <c r="I181" t="n">
+        <v>0</v>
+      </c>
+      <c r="J181" t="b">
+        <v>0</v>
+      </c>
+      <c r="K181" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6747,7 +7827,13 @@
       </c>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr"/>
-      <c r="I182" t="b">
+      <c r="I182" t="n">
+        <v>0</v>
+      </c>
+      <c r="J182" t="b">
+        <v>0</v>
+      </c>
+      <c r="K182" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6784,7 +7870,13 @@
       <c r="H183" t="n">
         <v>452.03</v>
       </c>
-      <c r="I183" t="b">
+      <c r="I183" t="n">
+        <v>4225665380</v>
+      </c>
+      <c r="J183" t="b">
+        <v>1</v>
+      </c>
+      <c r="K183" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6821,7 +7913,13 @@
       <c r="H184" t="n">
         <v>5549</v>
       </c>
-      <c r="I184" t="b">
+      <c r="I184" t="n">
+        <v>4130288076</v>
+      </c>
+      <c r="J184" t="b">
+        <v>1</v>
+      </c>
+      <c r="K184" t="b">
         <v>1</v>
       </c>
     </row>
@@ -6854,7 +7952,13 @@
       </c>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="inlineStr"/>
-      <c r="I185" t="b">
+      <c r="I185" t="n">
+        <v>0</v>
+      </c>
+      <c r="J185" t="b">
+        <v>0</v>
+      </c>
+      <c r="K185" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6887,7 +7991,13 @@
       </c>
       <c r="G186" t="inlineStr"/>
       <c r="H186" t="inlineStr"/>
-      <c r="I186" t="b">
+      <c r="I186" t="n">
+        <v>0</v>
+      </c>
+      <c r="J186" t="b">
+        <v>0</v>
+      </c>
+      <c r="K186" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6920,7 +8030,13 @@
       </c>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr"/>
-      <c r="I187" t="b">
+      <c r="I187" t="n">
+        <v>0</v>
+      </c>
+      <c r="J187" t="b">
+        <v>0</v>
+      </c>
+      <c r="K187" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6953,7 +8069,13 @@
       </c>
       <c r="G188" t="inlineStr"/>
       <c r="H188" t="inlineStr"/>
-      <c r="I188" t="b">
+      <c r="I188" t="n">
+        <v>0</v>
+      </c>
+      <c r="J188" t="b">
+        <v>0</v>
+      </c>
+      <c r="K188" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6990,7 +8112,13 @@
       <c r="H189" t="n">
         <v>14737.34</v>
       </c>
-      <c r="I189" t="b">
+      <c r="I189" t="n">
+        <v>7807769384</v>
+      </c>
+      <c r="J189" t="b">
+        <v>1</v>
+      </c>
+      <c r="K189" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7027,7 +8155,13 @@
       <c r="H190" t="n">
         <v>19804.2</v>
       </c>
-      <c r="I190" t="b">
+      <c r="I190" t="n">
+        <v>2775753386</v>
+      </c>
+      <c r="J190" t="b">
+        <v>1</v>
+      </c>
+      <c r="K190" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7060,7 +8194,13 @@
       </c>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="inlineStr"/>
-      <c r="I191" t="b">
+      <c r="I191" t="n">
+        <v>0</v>
+      </c>
+      <c r="J191" t="b">
+        <v>0</v>
+      </c>
+      <c r="K191" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7093,7 +8233,13 @@
       </c>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="inlineStr"/>
-      <c r="I192" t="b">
+      <c r="I192" t="n">
+        <v>0</v>
+      </c>
+      <c r="J192" t="b">
+        <v>0</v>
+      </c>
+      <c r="K192" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7130,7 +8276,13 @@
       <c r="H193" t="n">
         <v>51557.44</v>
       </c>
-      <c r="I193" t="b">
+      <c r="I193" t="n">
+        <v>4275042006</v>
+      </c>
+      <c r="J193" t="b">
+        <v>1</v>
+      </c>
+      <c r="K193" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7167,7 +8319,13 @@
       <c r="H194" t="n">
         <v>11304.33</v>
       </c>
-      <c r="I194" t="b">
+      <c r="I194" t="n">
+        <v>4091208039</v>
+      </c>
+      <c r="J194" t="b">
+        <v>1</v>
+      </c>
+      <c r="K194" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7204,7 +8362,13 @@
       <c r="H195" t="n">
         <v>32962.5</v>
       </c>
-      <c r="I195" t="b">
+      <c r="I195" t="n">
+        <v>2896232466</v>
+      </c>
+      <c r="J195" t="b">
+        <v>1</v>
+      </c>
+      <c r="K195" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7241,7 +8405,13 @@
       <c r="H196" t="n">
         <v>7260.69</v>
       </c>
-      <c r="I196" t="b">
+      <c r="I196" t="n">
+        <v>3191727173</v>
+      </c>
+      <c r="J196" t="b">
+        <v>1</v>
+      </c>
+      <c r="K196" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7278,7 +8448,13 @@
       <c r="H197" t="n">
         <v>11781.16</v>
       </c>
-      <c r="I197" t="b">
+      <c r="I197" t="n">
+        <v>32347249310</v>
+      </c>
+      <c r="J197" t="b">
+        <v>1</v>
+      </c>
+      <c r="K197" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7313,7 +8489,13 @@
         <v>91467726</v>
       </c>
       <c r="H198" t="inlineStr"/>
-      <c r="I198" t="b">
+      <c r="I198" t="n">
+        <v>11473410243</v>
+      </c>
+      <c r="J198" t="b">
+        <v>1</v>
+      </c>
+      <c r="K198" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7350,7 +8532,13 @@
       <c r="H199" t="n">
         <v>758.15</v>
       </c>
-      <c r="I199" t="b">
+      <c r="I199" t="n">
+        <v>8924116899</v>
+      </c>
+      <c r="J199" t="b">
+        <v>1</v>
+      </c>
+      <c r="K199" t="b">
         <v>1</v>
       </c>
     </row>
@@ -7383,7 +8571,13 @@
       </c>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="inlineStr"/>
-      <c r="I200" t="b">
+      <c r="I200" t="n">
+        <v>0</v>
+      </c>
+      <c r="J200" t="b">
+        <v>0</v>
+      </c>
+      <c r="K200" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7412,7 +8606,11 @@
       </c>
       <c r="G201" t="inlineStr"/>
       <c r="H201" t="inlineStr"/>
-      <c r="I201" t="b">
+      <c r="I201" t="inlineStr"/>
+      <c r="J201" t="b">
+        <v>0</v>
+      </c>
+      <c r="K201" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>